<commit_message>
Correción de context en extensiones
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-IdContacto.xlsx
+++ b/output/StructureDefinition-IdContacto.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-06-25T09:29:41-04:00</t>
+    <t>2024-06-26T18:33:17-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -135,7 +135,7 @@
     <t>Context</t>
   </si>
   <si>
-    <t>element:https://hl7chile.cl/fhir/ig/clcore/StructureDefinition/CorePacienteCl#Patient.contact</t>
+    <t>element:Patient.contact</t>
   </si>
   <si>
     <t>ID</t>

</xml_diff>